<commit_message>
Add passives to BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="94">
   <si>
     <t>Spur v1.0 BOM</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Rating</t>
-  </si>
-  <si>
     <t>Package</t>
   </si>
   <si>
@@ -55,19 +52,193 @@
     <t>Price @ Qty 100</t>
   </si>
   <si>
-    <t>Notes</t>
+    <t>C1, C2</t>
+  </si>
+  <si>
+    <t>Capacitor, ceramic, 6.3V</t>
+  </si>
+  <si>
+    <t>1u</t>
+  </si>
+  <si>
+    <t>0402</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>CL05A105KQ5NNNC</t>
+  </si>
+  <si>
+    <t>1276-1010-1-ND</t>
+  </si>
+  <si>
+    <t>C3, C8, C9, C10, C11</t>
+  </si>
+  <si>
+    <t>0.1u</t>
+  </si>
+  <si>
+    <t>CL05A104KQ5NNNC</t>
+  </si>
+  <si>
+    <t>1276-1442-1-ND</t>
+  </si>
+  <si>
+    <t>C4, C5</t>
+  </si>
+  <si>
+    <t>Capacitor, ceramic, 50V</t>
+  </si>
+  <si>
+    <t>4p</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>CC0402BRNPO9BN4R0</t>
+  </si>
+  <si>
+    <t>311-3705-1-ND</t>
+  </si>
+  <si>
+    <t>C6, C7</t>
+  </si>
+  <si>
+    <t>Capacitor, ceramic, 10V</t>
+  </si>
+  <si>
+    <t>4.7u</t>
+  </si>
+  <si>
+    <t>CL05A475MP5NRNC</t>
+  </si>
+  <si>
+    <t>1276-1482-1-ND</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Zener diode, ESD</t>
+  </si>
+  <si>
+    <t>ON Semi</t>
+  </si>
+  <si>
+    <t>NSPU3051N2T5G</t>
+  </si>
+  <si>
+    <t>NSPU3051N2T5GOSCT-ND</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>LED, green</t>
+  </si>
+  <si>
+    <t>Kingbright</t>
+  </si>
+  <si>
+    <t>APHHS1005CGCK</t>
+  </si>
+  <si>
+    <t>754-1101-1-ND</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>Diode array, ESD, 2 channel</t>
+  </si>
+  <si>
+    <t>SOT-886</t>
+  </si>
+  <si>
+    <t>Nexperia</t>
+  </si>
+  <si>
+    <t>PRTR5V0U2F,115</t>
+  </si>
+  <si>
+    <t>1727-4161-1-ND</t>
   </si>
   <si>
     <t>PCB1</t>
   </si>
   <si>
-    <t>Bare PCB</t>
+    <t>Bare PCB, 2 layer, 0.6mm, 1oz, ENIG</t>
+  </si>
+  <si>
+    <t>JLCPCB</t>
+  </si>
+  <si>
+    <t>R1, R3, R4, R5, R6, R7</t>
+  </si>
+  <si>
+    <t>Resistor, thick film, 1%, 1/16W</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>RC0402FR-0710KL</t>
+  </si>
+  <si>
+    <t>311-10.0KLRCT-ND</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>23K</t>
+  </si>
+  <si>
+    <t>RC0402FR-0722KL</t>
+  </si>
+  <si>
+    <t>311-22.0KLRCT-ND</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>Slide switch, SPDT</t>
+  </si>
+  <si>
+    <t>JS102000SAQN</t>
+  </si>
+  <si>
+    <t>C&amp;K</t>
+  </si>
+  <si>
+    <t>401-2005-1-ND</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>Linear regulator, adjustable, 150mA</t>
+  </si>
+  <si>
+    <t>SOT-353</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>MIC5377YC5-TR</t>
+  </si>
+  <si>
+    <t>576-3358-1-ND</t>
   </si>
   <si>
     <t>U2</t>
   </si>
   <si>
-    <t>SPI NOR flash 1MiB</t>
+    <t>Flash memory, NOR, SPI, 1MiB</t>
   </si>
   <si>
     <t>8-UDFN</t>
@@ -85,7 +256,7 @@
     <t>U3</t>
   </si>
   <si>
-    <t>STM32F4 128Kb flash</t>
+    <t>Microcontroller, 128KiB flash</t>
   </si>
   <si>
     <t>48-UFQFN</t>
@@ -100,64 +271,10 @@
     <t>497-17425-ND</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>LDO adj. 150mA</t>
-  </si>
-  <si>
-    <t>SOT-353</t>
-  </si>
-  <si>
-    <t>Microchip</t>
-  </si>
-  <si>
-    <t>MIC5377YC5-TR</t>
-  </si>
-  <si>
-    <t>576-3358-1-ND</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>ESD diode 2 CH</t>
-  </si>
-  <si>
-    <t>SOT-886</t>
-  </si>
-  <si>
-    <t>Nexperia</t>
-  </si>
-  <si>
-    <t>PRTR5V0U2F,115</t>
-  </si>
-  <si>
-    <t>1727-4161-1-ND</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>ESD zener diode</t>
-  </si>
-  <si>
-    <t>0402</t>
-  </si>
-  <si>
-    <t>ON Semi</t>
-  </si>
-  <si>
-    <t>NSPU3051N2T5G</t>
-  </si>
-  <si>
-    <t>NSPU3051N2T5GOSCT-ND</t>
-  </si>
-  <si>
     <t>Y1</t>
   </si>
   <si>
-    <t>24MHz crystal, Cl 12pF</t>
+    <t>Crystal, 24MHz, Cl=12pF</t>
   </si>
   <si>
     <t>4-SMD</t>
@@ -170,21 +287,6 @@
   </si>
   <si>
     <t>490-18289-1-ND</t>
-  </si>
-  <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>Slide switch SPDT</t>
-  </si>
-  <si>
-    <t>C&amp;K</t>
-  </si>
-  <si>
-    <t>JS102000SAQN</t>
-  </si>
-  <si>
-    <t>401-2005-1-ND</t>
   </si>
   <si>
     <t>Price @ Qty 1:</t>
@@ -198,8 +300,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00000"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00000"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -215,16 +317,16 @@
     </font>
     <font>
       <b/>
+    </font>
+    <font/>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font/>
-    <font>
-      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -254,37 +356,37 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -334,8 +436,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A2:N11" displayName="Table_1" id="1">
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A2:L18" displayName="Table_1" id="1">
+  <tableColumns count="12">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
     <tableColumn name="Column3" id="3"/>
@@ -348,8 +450,6 @@
     <tableColumn name="Column10" id="10"/>
     <tableColumn name="Column11" id="11"/>
     <tableColumn name="Column12" id="12"/>
-    <tableColumn name="Column13" id="13"/>
-    <tableColumn name="Column14" id="14"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -562,18 +662,16 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="5.14"/>
     <col customWidth="1" min="2" max="2" width="8.71"/>
-    <col customWidth="1" min="3" max="3" width="28.71"/>
+    <col customWidth="1" min="3" max="3" width="33.0"/>
     <col customWidth="1" min="4" max="4" width="6.14"/>
-    <col customWidth="1" min="5" max="5" width="7.0"/>
-    <col customWidth="1" min="6" max="6" width="10.43"/>
-    <col customWidth="1" min="7" max="7" width="14.43"/>
-    <col customWidth="1" min="8" max="8" width="23.0"/>
-    <col customWidth="1" min="9" max="9" width="31.0"/>
-    <col customWidth="1" min="10" max="10" width="17.71"/>
-    <col customWidth="1" min="11" max="11" width="13.43"/>
-    <col customWidth="1" min="12" max="12" width="19.86"/>
-    <col customWidth="1" min="13" max="13" width="15.57"/>
-    <col customWidth="1" min="14" max="14" width="7.29"/>
+    <col customWidth="1" min="5" max="5" width="15.14"/>
+    <col customWidth="1" min="6" max="6" width="13.14"/>
+    <col customWidth="1" min="7" max="7" width="23.0"/>
+    <col customWidth="1" min="8" max="8" width="31.0"/>
+    <col customWidth="1" min="9" max="9" width="17.71"/>
+    <col customWidth="1" min="10" max="10" width="13.43"/>
+    <col customWidth="1" min="11" max="11" width="19.86"/>
+    <col customWidth="1" min="12" max="12" width="15.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -618,168 +716,182 @@
       <c r="L2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="3">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="4"/>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="7">
+        <f t="shared" ref="J3:J9" si="1">A3*I3</f>
+        <v>0.2</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0.0087</v>
+      </c>
+      <c r="L3" s="7">
+        <f t="shared" ref="L3:L9" si="2">A3*K3</f>
+        <v>0.0174</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B4" s="6" t="s">
+        <v>5.0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="7" t="s">
-        <v>19</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="8">
-        <v>0.4</v>
-      </c>
-      <c r="K4" s="9">
-        <f t="shared" ref="K4:K10" si="1">A4*J4</f>
-        <v>0.4</v>
-      </c>
-      <c r="L4" s="10">
-        <v>0.3256</v>
-      </c>
-      <c r="M4" s="9">
-        <f t="shared" ref="M4:M10" si="2">A4*L4</f>
-        <v>0.3256</v>
-      </c>
-      <c r="N4" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0.0085</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.0425</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>23</v>
+        <v>2.0</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="7" t="s">
         <v>25</v>
       </c>
+      <c r="D5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="G5" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="8">
-        <v>4.96</v>
-      </c>
-      <c r="K5" s="9">
+        <v>29</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J5" s="7">
         <f t="shared" si="1"/>
-        <v>4.96</v>
-      </c>
-      <c r="L5" s="8">
-        <v>3.6469</v>
-      </c>
-      <c r="M5" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0.0176</v>
+      </c>
+      <c r="L5" s="7">
         <f t="shared" si="2"/>
-        <v>3.6469</v>
-      </c>
-      <c r="N5" s="4"/>
+        <v>0.0352</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="6" t="s">
+        <v>2.0</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="7" t="s">
+      <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="D6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="G6" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="8">
-        <v>0.26</v>
-      </c>
-      <c r="K6" s="9">
+      <c r="I6" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J6" s="7">
         <f t="shared" si="1"/>
-        <v>0.26</v>
-      </c>
-      <c r="L6" s="8">
         <v>0.2</v>
       </c>
-      <c r="M6" s="9">
+      <c r="K6" s="6">
+        <v>0.00336</v>
+      </c>
+      <c r="L6" s="7">
         <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-      <c r="N6" s="4"/>
+        <v>0.00672</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3">
         <v>1.0</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="7" t="s">
+      <c r="D7" s="8"/>
+      <c r="E7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -788,172 +900,416 @@
       <c r="H7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="8">
-        <v>0.49</v>
-      </c>
-      <c r="K7" s="9">
+      <c r="I7" s="6">
+        <v>0.36</v>
+      </c>
+      <c r="J7" s="7">
         <f t="shared" si="1"/>
-        <v>0.49</v>
-      </c>
-      <c r="L7" s="8">
-        <v>0.255</v>
-      </c>
-      <c r="M7" s="9">
+        <v>0.36</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0.1344</v>
+      </c>
+      <c r="L7" s="7">
         <f t="shared" si="2"/>
-        <v>0.255</v>
-      </c>
-      <c r="N7" s="4"/>
+        <v>0.1344</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3">
         <v>1.0</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="8"/>
+      <c r="E8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="11" t="s">
+      <c r="G8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J8" s="8">
-        <v>0.36</v>
-      </c>
-      <c r="K8" s="9">
+      <c r="I8" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="J8" s="7">
         <f t="shared" si="1"/>
-        <v>0.36</v>
-      </c>
-      <c r="L8" s="8">
-        <v>0.1344</v>
-      </c>
-      <c r="M8" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.1645</v>
+      </c>
+      <c r="L8" s="7">
         <f t="shared" si="2"/>
-        <v>0.1344</v>
-      </c>
-      <c r="N8" s="4"/>
+        <v>0.1645</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="3">
         <v>1.0</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="F9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J9" s="8">
-        <v>0.44</v>
-      </c>
-      <c r="K9" s="9">
+      <c r="I9" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="J9" s="7">
         <f t="shared" si="1"/>
-        <v>0.44</v>
-      </c>
-      <c r="L9" s="8">
-        <v>0.291</v>
-      </c>
-      <c r="M9" s="9">
+        <v>0.49</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0.255</v>
+      </c>
+      <c r="L9" s="7">
         <f t="shared" si="2"/>
-        <v>0.291</v>
-      </c>
-      <c r="N9" s="4"/>
+        <v>0.255</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3">
         <v>1.0</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="E11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="J10" s="8">
+      <c r="H11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" ref="J11:J17" si="3">A11*I11</f>
+        <v>0.6</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0.0058</v>
+      </c>
+      <c r="L11" s="7">
+        <f t="shared" ref="L11:L17" si="4">A11*K11</f>
+        <v>0.0348</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0.0058</v>
+      </c>
+      <c r="L12" s="7">
+        <f t="shared" si="4"/>
+        <v>0.0058</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="6">
         <v>0.71</v>
       </c>
-      <c r="K10" s="9">
-        <f t="shared" si="1"/>
+      <c r="J13" s="7">
+        <f t="shared" si="3"/>
         <v>0.71</v>
       </c>
-      <c r="L10" s="8">
+      <c r="K13" s="6">
         <v>0.5696</v>
       </c>
-      <c r="M10" s="9">
-        <f t="shared" si="2"/>
+      <c r="L13" s="7">
+        <f t="shared" si="4"/>
         <v>0.5696</v>
       </c>
-      <c r="N10" s="4"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="K11" s="14">
-        <f>SUM(K4:K10)</f>
-        <v>7.62</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="M11" s="14">
-        <f>SUM(M4:M10)</f>
-        <v>5.4225</v>
-      </c>
-      <c r="N11" s="4"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0.26</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="3"/>
+        <v>0.26</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="L14" s="7">
+        <f t="shared" si="4"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0.3256</v>
+      </c>
+      <c r="L15" s="7">
+        <f t="shared" si="4"/>
+        <v>0.3256</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I16" s="6">
+        <v>4.96</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="3"/>
+        <v>4.96</v>
+      </c>
+      <c r="K16" s="6">
+        <v>3.6469</v>
+      </c>
+      <c r="L16" s="7">
+        <f t="shared" si="4"/>
+        <v>3.6469</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I17" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="3"/>
+        <v>0.44</v>
+      </c>
+      <c r="K17" s="6">
+        <v>0.291</v>
+      </c>
+      <c r="L17" s="7">
+        <f t="shared" si="4"/>
+        <v>0.291</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="J18" s="14">
+        <f>SUM(J3:J17)</f>
+        <v>9.82</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="L18" s="14">
+        <f>SUM(L3:L17)</f>
+        <v>5.72942</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Add PCB to BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -377,8 +377,8 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -746,14 +746,14 @@
         <v>0.1</v>
       </c>
       <c r="J3" s="7">
-        <f t="shared" ref="J3:J9" si="1">A3*I3</f>
+        <f t="shared" ref="J3:J17" si="1">A3*I3</f>
         <v>0.2</v>
       </c>
       <c r="K3" s="6">
         <v>0.0087</v>
       </c>
       <c r="L3" s="7">
-        <f t="shared" ref="L3:L9" si="2">A3*K3</f>
+        <f t="shared" ref="L3:L17" si="2">A3*K3</f>
         <v>0.0174</v>
       </c>
     </row>
@@ -1008,10 +1008,22 @@
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
+      <c r="I10" s="11">
+        <f>18/5</f>
+        <v>3.6</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="1"/>
+        <v>3.6</v>
+      </c>
+      <c r="K10" s="11">
+        <f>49.5/100</f>
+        <v>0.495</v>
+      </c>
+      <c r="L10" s="7">
+        <f t="shared" si="2"/>
+        <v>0.495</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="3">
@@ -1042,14 +1054,14 @@
         <v>0.1</v>
       </c>
       <c r="J11" s="7">
-        <f t="shared" ref="J11:J17" si="3">A11*I11</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="K11" s="6">
         <v>0.0058</v>
       </c>
       <c r="L11" s="7">
-        <f t="shared" ref="L11:L17" si="4">A11*K11</f>
+        <f t="shared" si="2"/>
         <v>0.0348</v>
       </c>
     </row>
@@ -1082,14 +1094,14 @@
         <v>0.1</v>
       </c>
       <c r="J12" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="K12" s="6">
         <v>0.0058</v>
       </c>
       <c r="L12" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.0058</v>
       </c>
     </row>
@@ -1120,14 +1132,14 @@
         <v>0.71</v>
       </c>
       <c r="J13" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.71</v>
       </c>
       <c r="K13" s="6">
         <v>0.5696</v>
       </c>
       <c r="L13" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.5696</v>
       </c>
     </row>
@@ -1158,14 +1170,14 @@
         <v>0.26</v>
       </c>
       <c r="J14" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.26</v>
       </c>
       <c r="K14" s="6">
         <v>0.2</v>
       </c>
       <c r="L14" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
     </row>
@@ -1196,14 +1208,14 @@
         <v>0.4</v>
       </c>
       <c r="J15" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="K15" s="6">
         <v>0.3256</v>
       </c>
       <c r="L15" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.3256</v>
       </c>
     </row>
@@ -1234,14 +1246,14 @@
         <v>4.96</v>
       </c>
       <c r="J16" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>4.96</v>
       </c>
       <c r="K16" s="6">
         <v>3.6469</v>
       </c>
       <c r="L16" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3.6469</v>
       </c>
     </row>
@@ -1272,14 +1284,14 @@
         <v>0.44</v>
       </c>
       <c r="J17" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.44</v>
       </c>
       <c r="K17" s="6">
         <v>0.291</v>
       </c>
       <c r="L17" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.291</v>
       </c>
     </row>
@@ -1297,14 +1309,14 @@
       </c>
       <c r="J18" s="14">
         <f>SUM(J3:J17)</f>
-        <v>9.82</v>
+        <v>13.42</v>
       </c>
       <c r="K18" s="13" t="s">
         <v>93</v>
       </c>
       <c r="L18" s="14">
         <f>SUM(L3:L17)</f>
-        <v>5.72942</v>
+        <v>6.22442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove pull-ups, bulk cap from BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="89">
   <si>
     <t>Spur v1.0 BOM</t>
   </si>
@@ -73,7 +73,7 @@
     <t>1276-1010-1-ND</t>
   </si>
   <si>
-    <t>C3, C8, C9, C10, C11</t>
+    <t>C3, C7, C8, C9, C10</t>
   </si>
   <si>
     <t>0.1u</t>
@@ -103,7 +103,7 @@
     <t>311-3705-1-ND</t>
   </si>
   <si>
-    <t>C6, C7</t>
+    <t>C6</t>
   </si>
   <si>
     <t>Capacitor, ceramic, 10V</t>
@@ -136,21 +136,6 @@
     <t>D2</t>
   </si>
   <si>
-    <t>LED, green</t>
-  </si>
-  <si>
-    <t>Kingbright</t>
-  </si>
-  <si>
-    <t>APHHS1005CGCK</t>
-  </si>
-  <si>
-    <t>754-1101-1-ND</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
     <t>Diode array, ESD, 2 channel</t>
   </si>
   <si>
@@ -175,7 +160,7 @@
     <t>JLCPCB</t>
   </si>
   <si>
-    <t>R1, R3, R4, R5, R6, R7</t>
+    <t>R2, R3</t>
   </si>
   <si>
     <t>Resistor, thick film, 1%, 1/16W</t>
@@ -190,7 +175,7 @@
     <t>311-10.0KLRCT-ND</t>
   </si>
   <si>
-    <t>R2</t>
+    <t>R1</t>
   </si>
   <si>
     <t>23K</t>
@@ -303,7 +288,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00000"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -317,17 +302,14 @@
     </font>
     <font>
       <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <b/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -365,8 +347,11 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -377,16 +362,13 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -436,7 +418,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A2:L18" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A2:L17" displayName="Table_1" id="1">
   <tableColumns count="12">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -746,14 +728,14 @@
         <v>0.1</v>
       </c>
       <c r="J3" s="7">
-        <f t="shared" ref="J3:J17" si="1">A3*I3</f>
+        <f t="shared" ref="J3:J16" si="1">A3*I3</f>
         <v>0.2</v>
       </c>
       <c r="K3" s="6">
         <v>0.0087</v>
       </c>
       <c r="L3" s="7">
-        <f t="shared" ref="L3:L17" si="2">A3*K3</f>
+        <f t="shared" ref="L3:L16" si="2">A3*K3</f>
         <v>0.0174</v>
       </c>
     </row>
@@ -761,7 +743,7 @@
       <c r="A4" s="3">
         <v>5.0</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -838,10 +820,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -867,14 +849,14 @@
       </c>
       <c r="J6" s="7">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="K6" s="6">
         <v>0.00336</v>
       </c>
       <c r="L6" s="7">
         <f t="shared" si="2"/>
-        <v>0.00672</v>
+        <v>0.00336</v>
       </c>
     </row>
     <row r="7">
@@ -887,7 +869,7 @@
       <c r="C7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="5" t="s">
         <v>16</v>
       </c>
@@ -919,38 +901,38 @@
       <c r="A8" s="3">
         <v>1.0</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="9"/>
       <c r="E8" s="5" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I8" s="6">
-        <v>0.4</v>
+        <v>0.49</v>
       </c>
       <c r="J8" s="7">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.49</v>
       </c>
       <c r="K8" s="6">
-        <v>0.1645</v>
+        <v>0.255</v>
       </c>
       <c r="L8" s="7">
         <f t="shared" si="2"/>
-        <v>0.1645</v>
+        <v>0.255</v>
       </c>
     </row>
     <row r="9">
@@ -958,85 +940,87 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="5" t="s">
         <v>47</v>
       </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="10"/>
       <c r="F9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
       <c r="I9" s="6">
-        <v>0.49</v>
+        <f>18/5</f>
+        <v>3.6</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" si="1"/>
-        <v>0.49</v>
+        <v>3.6</v>
       </c>
       <c r="K9" s="6">
-        <v>0.255</v>
+        <f>49.5/100</f>
+        <v>0.495</v>
       </c>
       <c r="L9" s="7">
         <f t="shared" si="2"/>
-        <v>0.255</v>
+        <v>0.495</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="E10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="11">
-        <f>18/5</f>
-        <v>3.6</v>
+      <c r="I10" s="6">
+        <v>0.1</v>
       </c>
       <c r="J10" s="7">
         <f t="shared" si="1"/>
-        <v>3.6</v>
-      </c>
-      <c r="K10" s="11">
-        <f>49.5/100</f>
-        <v>0.495</v>
+        <v>0.2</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0.0058</v>
       </c>
       <c r="L10" s="7">
         <f t="shared" si="2"/>
-        <v>0.495</v>
+        <v>0.0116</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3">
-        <v>6.0</v>
-      </c>
-      <c r="B11" s="3" t="s">
+        <v>1.0</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>16</v>
@@ -1045,24 +1029,24 @@
         <v>27</v>
       </c>
       <c r="G11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="I11" s="6">
         <v>0.1</v>
       </c>
       <c r="J11" s="7">
         <f t="shared" si="1"/>
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="K11" s="6">
         <v>0.0058</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" si="2"/>
-        <v>0.0348</v>
+        <v>0.0058</v>
       </c>
     </row>
     <row r="12">
@@ -1070,39 +1054,37 @@
         <v>1.0</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="9"/>
+      <c r="E12" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="F12" s="3" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>62</v>
       </c>
       <c r="I12" s="6">
-        <v>0.1</v>
+        <v>0.71</v>
       </c>
       <c r="J12" s="7">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.71</v>
       </c>
       <c r="K12" s="6">
-        <v>0.0058</v>
+        <v>0.5696</v>
       </c>
       <c r="L12" s="7">
         <f t="shared" si="2"/>
-        <v>0.0058</v>
+        <v>0.5696</v>
       </c>
     </row>
     <row r="13">
@@ -1115,32 +1097,32 @@
       <c r="C13" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="12" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="5" t="s">
         <v>65</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>66</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I13" s="6">
-        <v>0.71</v>
+        <v>0.26</v>
       </c>
       <c r="J13" s="7">
         <f t="shared" si="1"/>
-        <v>0.71</v>
+        <v>0.26</v>
       </c>
       <c r="K13" s="6">
-        <v>0.5696</v>
+        <v>0.2</v>
       </c>
       <c r="L13" s="7">
         <f t="shared" si="2"/>
-        <v>0.5696</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="14">
@@ -1148,37 +1130,37 @@
         <v>1.0</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="8"/>
+        <v>70</v>
+      </c>
+      <c r="D14" s="9"/>
       <c r="E14" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I14" s="6">
-        <v>0.26</v>
+        <v>0.4</v>
       </c>
       <c r="J14" s="7">
         <f t="shared" si="1"/>
-        <v>0.26</v>
+        <v>0.4</v>
       </c>
       <c r="K14" s="6">
-        <v>0.2</v>
+        <v>0.3256</v>
       </c>
       <c r="L14" s="7">
         <f t="shared" si="2"/>
-        <v>0.2</v>
+        <v>0.3256</v>
       </c>
     </row>
     <row r="15">
@@ -1186,37 +1168,37 @@
         <v>1.0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="8"/>
+        <v>76</v>
+      </c>
+      <c r="D15" s="9"/>
       <c r="E15" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I15" s="6">
-        <v>0.4</v>
+        <v>4.96</v>
       </c>
       <c r="J15" s="7">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>4.96</v>
       </c>
       <c r="K15" s="6">
-        <v>0.3256</v>
+        <v>3.6469</v>
       </c>
       <c r="L15" s="7">
         <f t="shared" si="2"/>
-        <v>0.3256</v>
+        <v>3.6469</v>
       </c>
     </row>
     <row r="16">
@@ -1224,99 +1206,61 @@
         <v>1.0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D16" s="8"/>
+        <v>82</v>
+      </c>
+      <c r="D16" s="9"/>
       <c r="E16" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I16" s="6">
-        <v>4.96</v>
+        <v>0.44</v>
       </c>
       <c r="J16" s="7">
         <f t="shared" si="1"/>
-        <v>4.96</v>
+        <v>0.44</v>
       </c>
       <c r="K16" s="6">
-        <v>3.6469</v>
+        <v>0.291</v>
       </c>
       <c r="L16" s="7">
         <f t="shared" si="2"/>
-        <v>3.6469</v>
+        <v>0.291</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="A17" s="3"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="5" t="s">
+      <c r="J17" s="14">
+        <f>SUM(J3:J16)</f>
+        <v>12.52</v>
+      </c>
+      <c r="K17" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I17" s="6">
-        <v>0.44</v>
-      </c>
-      <c r="J17" s="7">
-        <f t="shared" si="1"/>
-        <v>0.44</v>
-      </c>
-      <c r="K17" s="6">
-        <v>0.291</v>
-      </c>
-      <c r="L17" s="7">
-        <f t="shared" si="2"/>
-        <v>0.291</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="3"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="J18" s="14">
-        <f>SUM(J3:J17)</f>
-        <v>13.42</v>
-      </c>
-      <c r="K18" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="L18" s="14">
-        <f>SUM(L3:L17)</f>
-        <v>6.22442</v>
+      <c r="L17" s="14">
+        <f>SUM(L3:L16)</f>
+        <v>6.03336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>